<commit_message>
update R script with framework to estimate offsets and modify driver files WITHOUT EXCEL!!
</commit_message>
<xml_diff>
--- a/Teleconnections/Variable_Name_Metadata.xlsx
+++ b/Teleconnections/Variable_Name_Metadata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KFarrell\Desktop\R\ProjectEDDIE\CrossScale Emergence\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KJF\Desktop\R\MacrosystemsEDDIE\Teleconnections\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="45">
   <si>
     <t>File name</t>
   </si>
@@ -105,18 +105,6 @@
   </si>
   <si>
     <t>TEMP</t>
-  </si>
-  <si>
-    <t>OGM_don</t>
-  </si>
-  <si>
-    <t>NIT_nit</t>
-  </si>
-  <si>
-    <t>NIT_amm</t>
-  </si>
-  <si>
-    <t>PHS_frp</t>
   </si>
   <si>
     <t>outflow.csv</t>
@@ -160,18 +148,6 @@
     <t>water temperature</t>
   </si>
   <si>
-    <t>dissolved organic nitrogen concentration in inflow water</t>
-  </si>
-  <si>
-    <t>nitrate concentration in inflow water</t>
-  </si>
-  <si>
-    <t>ammonium concentration in inflow water</t>
-  </si>
-  <si>
-    <t>filterable reactive phosphorus concentration in inflow water</t>
-  </si>
-  <si>
     <t>shortwave radiation</t>
   </si>
   <si>
@@ -208,38 +184,6 @@
     <t>parts per thousand</t>
   </si>
   <si>
-    <r>
-      <t>mmol N/m</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>3</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>mmol P/m</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>3</t>
-    </r>
-  </si>
-  <si>
     <t>Unit Conversion Notes</t>
   </si>
   <si>
@@ -250,32 +194,6 @@
   </si>
   <si>
     <t>convert from cubic feet per second by multiplying by 0.0283</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">convert </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>from</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> mg/L by multiplying by 32.29</t>
-    </r>
   </si>
 </sst>
 </file>
@@ -353,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -371,11 +289,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -690,10 +606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,7 +643,7 @@
         <v>20</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -741,9 +657,9 @@
         <v>15</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E2" s="10">
+        <v>39</v>
+      </c>
+      <c r="E2" s="9">
         <v>36587</v>
       </c>
     </row>
@@ -755,7 +671,7 @@
         <v>9</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -764,7 +680,7 @@
         <v>-2.5139999999999998</v>
       </c>
       <c r="F3" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
@@ -775,7 +691,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
@@ -784,7 +700,7 @@
         <v>308.887</v>
       </c>
       <c r="F4" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -804,7 +720,7 @@
         <v>20.05</v>
       </c>
       <c r="F5" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -824,7 +740,7 @@
         <v>38.619999999999997</v>
       </c>
       <c r="F6" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -864,10 +780,10 @@
         <v>5.9199999999999997E-4</v>
       </c>
       <c r="F8" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G8" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -887,7 +803,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="G9" s="5"/>
     </row>
@@ -902,9 +818,9 @@
         <v>15</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" s="10">
+        <v>39</v>
+      </c>
+      <c r="E10" s="9">
         <v>36587</v>
       </c>
     </row>
@@ -916,7 +832,7 @@
         <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>5</v>
@@ -925,10 +841,10 @@
         <v>2.38</v>
       </c>
       <c r="F11" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G11" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -939,7 +855,7 @@
         <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>5</v>
@@ -948,7 +864,7 @@
         <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -968,129 +884,45 @@
         <v>17.2</v>
       </c>
       <c r="F13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>49</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14">
-        <v>92.601500000000001</v>
-      </c>
-      <c r="F14" t="s">
-        <v>37</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="9">
+        <v>36587</v>
+      </c>
+      <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" t="s">
         <v>5</v>
       </c>
       <c r="E15">
-        <v>926.01530000000002</v>
+        <v>1.41</v>
       </c>
       <c r="F15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" t="s">
         <v>29</v>
-      </c>
-      <c r="C16" t="s">
-        <v>49</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E16">
-        <v>14.084899999999999</v>
-      </c>
-      <c r="F16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17" s="5">
-        <v>0.79179641999999995</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="H17" s="11"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E18" s="10">
-        <v>36587</v>
-      </c>
-      <c r="F18" s="4"/>
-    </row>
-    <row r="19" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" t="s">
-        <v>5</v>
-      </c>
-      <c r="E19">
-        <v>1.41</v>
-      </c>
-      <c r="F19" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>